<commit_message>
trying to sort out rotated text
</commit_message>
<xml_diff>
--- a/source/DocSource/SmokeTestArch.xlsx
+++ b/source/DocSource/SmokeTestArch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\dasblog-core\source\DocSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA228277-225B-498B-8970-59E6324B5986}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB63DAD5-7EEF-4D8E-A082-C55FC639CF61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="6705" xr2:uid="{A316D3C8-570E-4CC4-8439-B962472ED26E}"/>
   </bookViews>
@@ -209,7 +209,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>FirefoxDriver.dll</a:t>
+            <a:t>Driver</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1665,7 +1665,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>